<commit_message>
fix google map bug,delete not use file,arrange route
</commit_message>
<xml_diff>
--- a/backend/init_data.xlsx
+++ b/backend/init_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="416">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -1636,6 +1636,9 @@
     <t xml:space="preserve">remark</t>
   </si>
   <si>
+    <t xml:space="preserve">id_photo</t>
+  </si>
+  <si>
     <t xml:space="preserve">With a background in contemporary dance, My style of teaching focuses on awareness of movement and the connection between the body and mind.  Drawn to yoga’s power to create harmonic balance and still the mind, I have a passion for passing on what inspires me to others.</t>
   </si>
   <si>
@@ -1652,6 +1655,9 @@
   </si>
   <si>
     <t xml:space="preserve">accept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id.jpeg</t>
   </si>
   <si>
     <t xml:space="preserve">I have  pursued my education in a variety of Yoga styles such as Hatha, Ashtanga, Vinyasa, Yoga Therapy and Yin yoga, completing a total of 1000hrs of Teacher Training in India. As well as my Indian education, I have studied with top class teachers in London, developing an understanding and creating a style that binds the best of both, the traditional ancient eastern lineage and the modern scientific western approach.</t>
@@ -2005,11 +2011,11 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="176" zoomScaleNormal="176" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="176" zoomScaleNormal="176" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
@@ -2236,7 +2242,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.5"/>
   </cols>
@@ -2283,13 +2289,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.8"/>
@@ -2324,28 +2330,34 @@
       <c r="H1" s="0" t="s">
         <v>373</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2353,22 +2365,25 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>381</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="283.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2376,22 +2391,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,22 +2417,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>384</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -2439,7 +2460,7 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2449,10 +2470,10 @@
         <v>122</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,7 +2515,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +2529,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,7 +2557,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2571,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2613,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="83.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2641,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,7 +2655,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,7 +2669,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2662,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,7 +2697,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="83.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,7 +2711,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,7 +2725,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,7 +2739,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="71.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,7 +2753,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,7 +2767,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="60.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2760,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2795,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,7 +2809,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2813,7 +2834,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.97"/>
   </cols>
@@ -2976,7 +2997,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.83"/>
@@ -3875,7 +3896,7 @@
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -4265,7 +4286,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4333,7 +4354,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.07"/>
@@ -4995,7 +5016,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -6337,7 +6358,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -6399,7 +6420,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.56"/>

</xml_diff>

<commit_message>
add readme and amend init data excel file
</commit_message>
<xml_diff>
--- a/backend/init_data.xlsx
+++ b/backend/init_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" state="visible" r:id="rId2"/>
@@ -1770,7 +1770,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1795,6 +1795,13 @@
     </font>
     <font>
       <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -1869,7 +1876,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1882,6 +1889,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1890,7 +1901,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1898,11 +1909,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2011,11 +2022,11 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="176" zoomScaleNormal="176" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="176" zoomScaleNormal="176" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
@@ -2141,7 +2152,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2242,7 +2253,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.5"/>
   </cols>
@@ -2291,11 +2302,11 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F21" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.8"/>
@@ -2338,16 +2349,16 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>378</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -2364,16 +2375,16 @@
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>382</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>378</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -2390,7 +2401,7 @@
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>384</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -2399,7 +2410,7 @@
       <c r="D4" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>378</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -2425,7 +2436,7 @@
       <c r="D5" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>378</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -2460,7 +2471,7 @@
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2500,7 +2511,7 @@
       <c r="C3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>393</v>
       </c>
     </row>
@@ -2514,7 +2525,7 @@
       <c r="C4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>394</v>
       </c>
     </row>
@@ -2528,7 +2539,7 @@
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>395</v>
       </c>
     </row>
@@ -2542,7 +2553,7 @@
       <c r="C6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>396</v>
       </c>
     </row>
@@ -2556,7 +2567,7 @@
       <c r="C7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>397</v>
       </c>
     </row>
@@ -2570,7 +2581,7 @@
       <c r="C8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>398</v>
       </c>
     </row>
@@ -2584,7 +2595,7 @@
       <c r="C9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>399</v>
       </c>
     </row>
@@ -2598,7 +2609,7 @@
       <c r="C10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>400</v>
       </c>
     </row>
@@ -2612,7 +2623,7 @@
       <c r="C11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>401</v>
       </c>
     </row>
@@ -2626,7 +2637,7 @@
       <c r="C12" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>402</v>
       </c>
     </row>
@@ -2640,7 +2651,7 @@
       <c r="C13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>403</v>
       </c>
     </row>
@@ -2654,7 +2665,7 @@
       <c r="C14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>404</v>
       </c>
     </row>
@@ -2668,7 +2679,7 @@
       <c r="C15" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>405</v>
       </c>
     </row>
@@ -2682,7 +2693,7 @@
       <c r="C16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>406</v>
       </c>
     </row>
@@ -2696,7 +2707,7 @@
       <c r="C17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>407</v>
       </c>
     </row>
@@ -2710,7 +2721,7 @@
       <c r="C18" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>408</v>
       </c>
     </row>
@@ -2724,7 +2735,7 @@
       <c r="C19" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -2738,7 +2749,7 @@
       <c r="C20" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>410</v>
       </c>
     </row>
@@ -2752,7 +2763,7 @@
       <c r="C21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>411</v>
       </c>
     </row>
@@ -2766,7 +2777,7 @@
       <c r="C22" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>412</v>
       </c>
     </row>
@@ -2780,7 +2791,7 @@
       <c r="C23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>413</v>
       </c>
     </row>
@@ -2794,7 +2805,7 @@
       <c r="C24" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>414</v>
       </c>
     </row>
@@ -2834,7 +2845,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.97"/>
   </cols>
@@ -2848,7 +2859,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2856,7 +2867,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -2864,7 +2875,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -2872,7 +2883,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -2880,7 +2891,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -2888,7 +2899,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -2896,7 +2907,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -2904,7 +2915,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -2912,7 +2923,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -2920,7 +2931,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -2928,7 +2939,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -2936,7 +2947,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -2944,7 +2955,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -2952,7 +2963,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -2960,7 +2971,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -2997,14 +3008,14 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -3034,7 +3045,7 @@
       <c r="H1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -3046,13 +3057,13 @@
       <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>60</v>
       </c>
       <c r="P1" s="0" t="s">
@@ -3075,13 +3086,13 @@
       <c r="E2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -3093,13 +3104,13 @@
       <c r="L2" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3119,13 +3130,13 @@
       <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -3137,13 +3148,13 @@
       <c r="L3" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3163,13 +3174,13 @@
       <c r="E4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -3181,13 +3192,13 @@
       <c r="L4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3207,7 +3218,7 @@
       <c r="E5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -3216,7 +3227,7 @@
       <c r="H5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -3228,13 +3239,13 @@
       <c r="L5" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P5" s="0" t="s">
@@ -3257,7 +3268,7 @@
       <c r="E6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -3266,7 +3277,7 @@
       <c r="H6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -3278,13 +3289,13 @@
       <c r="L6" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="P6" s="0" t="s">
@@ -3307,7 +3318,7 @@
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -3316,7 +3327,7 @@
       <c r="H7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -3328,13 +3339,13 @@
       <c r="L7" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P7" s="0" t="s">
@@ -3357,13 +3368,13 @@
       <c r="E8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -3375,13 +3386,13 @@
       <c r="L8" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3401,13 +3412,13 @@
       <c r="E9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -3419,13 +3430,13 @@
       <c r="L9" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3445,7 +3456,7 @@
       <c r="E10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -3454,7 +3465,7 @@
       <c r="H10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -3466,13 +3477,13 @@
       <c r="L10" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P10" s="0" t="s">
@@ -3495,7 +3506,7 @@
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -3504,7 +3515,7 @@
       <c r="H11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -3516,13 +3527,13 @@
       <c r="L11" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="5" t="s">
         <v>70</v>
       </c>
       <c r="P11" s="0" t="s">
@@ -3545,7 +3556,7 @@
       <c r="E12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -3554,7 +3565,7 @@
       <c r="H12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -3566,13 +3577,13 @@
       <c r="L12" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P12" s="0" t="s">
@@ -3595,7 +3606,7 @@
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -3604,7 +3615,7 @@
       <c r="H13" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -3616,13 +3627,13 @@
       <c r="L13" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="5" t="s">
         <v>70</v>
       </c>
       <c r="P13" s="0" t="s">
@@ -3645,7 +3656,7 @@
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -3654,7 +3665,7 @@
       <c r="H14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -3666,13 +3677,13 @@
       <c r="L14" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P14" s="0" t="s">
@@ -3695,7 +3706,7 @@
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -3704,7 +3715,7 @@
       <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -3716,13 +3727,13 @@
       <c r="L15" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P15" s="0" t="s">
@@ -3745,7 +3756,7 @@
       <c r="E16" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -3754,7 +3765,7 @@
       <c r="H16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -3766,13 +3777,13 @@
       <c r="L16" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="5" t="s">
         <v>80</v>
       </c>
       <c r="P16" s="0" t="s">
@@ -3784,90 +3795,90 @@
       <c r="J17" s="1"/>
       <c r="K17" s="2"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="2"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="2"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="2"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="2"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="2"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="2"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="2"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="2"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3896,7 +3907,7 @@
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -4286,7 +4297,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4354,7 +4365,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.07"/>
@@ -4375,462 +4386,462 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="30.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="45.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="4" t="n">
         <v>250</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="3"/>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="4" t="n">
         <v>128</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="3"/>
+      <c r="D13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="30.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="3"/>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="3"/>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="30.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="D16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="3"/>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="D18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="30.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="30.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="3"/>
+      <c r="D21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="3"/>
+      <c r="D22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="30.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="D23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="50.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="4" t="n">
         <v>395</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3"/>
+      <c r="D24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="4" t="n">
         <v>393</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="4" t="n">
         <v>391</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="3"/>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="4" t="n">
         <v>388</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
+      <c r="D27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="99.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="4" t="n">
         <v>389</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
+      <c r="D28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="4" t="n">
         <v>392</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="3"/>
+      <c r="D29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="4" t="n">
         <v>390</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="3"/>
+      <c r="D30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="4" t="n">
         <v>387</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="3"/>
+      <c r="D31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5012,11 +5023,11 @@
   </sheetPr>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -5049,7 +5060,7 @@
       <c r="I1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5545,7 +5556,7 @@
       <c r="E30" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="4" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5562,7 +5573,7 @@
       <c r="E31" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="4" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5580,7 +5591,7 @@
       <c r="E32" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="4" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5597,7 +5608,7 @@
       <c r="E33" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="4" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5614,7 +5625,7 @@
       <c r="E34" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="4" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5631,7 +5642,7 @@
       <c r="E35" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="4" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5648,7 +5659,7 @@
       <c r="E36" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="4" t="s">
         <v>254</v>
       </c>
     </row>
@@ -5665,7 +5676,7 @@
       <c r="E37" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="4" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5682,7 +5693,7 @@
       <c r="E38" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="4" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5699,7 +5710,7 @@
       <c r="E39" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="4" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5716,7 +5727,7 @@
       <c r="E40" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="4" t="s">
         <v>258</v>
       </c>
     </row>
@@ -5733,7 +5744,7 @@
       <c r="E41" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="4" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5750,7 +5761,7 @@
       <c r="E42" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="4" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5767,7 +5778,7 @@
       <c r="E43" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="4" t="s">
         <v>261</v>
       </c>
     </row>
@@ -5784,7 +5795,7 @@
       <c r="E44" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="4" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5801,7 +5812,7 @@
       <c r="E45" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="4" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5818,7 +5829,7 @@
       <c r="E46" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="4" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5835,7 +5846,7 @@
       <c r="E47" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="4" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5852,7 +5863,7 @@
       <c r="E48" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="4" t="s">
         <v>266</v>
       </c>
     </row>
@@ -5869,7 +5880,7 @@
       <c r="E49" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="4" t="s">
         <v>267</v>
       </c>
     </row>
@@ -5886,7 +5897,7 @@
       <c r="E50" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="4" t="s">
         <v>268</v>
       </c>
     </row>
@@ -5903,7 +5914,7 @@
       <c r="E51" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="4" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5920,7 +5931,7 @@
       <c r="E52" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="4" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5937,7 +5948,7 @@
       <c r="E53" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="4" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5954,7 +5965,7 @@
       <c r="E54" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" s="4" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5971,7 +5982,7 @@
       <c r="E55" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="4" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5988,7 +5999,7 @@
       <c r="E56" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="4" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6006,7 +6017,7 @@
       <c r="E57" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="4" t="s">
         <v>275</v>
       </c>
     </row>
@@ -6023,7 +6034,7 @@
       <c r="E58" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F58" s="4" t="s">
         <v>276</v>
       </c>
     </row>
@@ -6040,7 +6051,7 @@
       <c r="E59" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="4" t="s">
         <v>277</v>
       </c>
     </row>
@@ -6057,7 +6068,7 @@
       <c r="E60" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="4" t="s">
         <v>278</v>
       </c>
     </row>
@@ -6074,7 +6085,7 @@
       <c r="E61" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="4" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6091,7 +6102,7 @@
       <c r="E62" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="4" t="s">
         <v>280</v>
       </c>
     </row>
@@ -6108,7 +6119,7 @@
       <c r="E63" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="4" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6125,7 +6136,7 @@
       <c r="E64" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="4" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6142,7 +6153,7 @@
       <c r="E65" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F65" s="4" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6159,7 +6170,7 @@
       <c r="E66" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="4" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6176,7 +6187,7 @@
       <c r="E67" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="4" t="s">
         <v>285</v>
       </c>
     </row>
@@ -6193,7 +6204,7 @@
       <c r="E68" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="4" t="s">
         <v>286</v>
       </c>
     </row>
@@ -6210,7 +6221,7 @@
       <c r="E69" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" s="4" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6227,7 +6238,7 @@
       <c r="E70" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F70" s="4" t="s">
         <v>288</v>
       </c>
     </row>
@@ -6244,7 +6255,7 @@
       <c r="E71" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F71" s="4" t="s">
         <v>289</v>
       </c>
     </row>
@@ -6261,7 +6272,7 @@
       <c r="E72" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" s="4" t="s">
         <v>290</v>
       </c>
     </row>
@@ -6278,7 +6289,7 @@
       <c r="E73" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="F73" s="4" t="s">
         <v>291</v>
       </c>
     </row>
@@ -6295,7 +6306,7 @@
       <c r="E74" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F74" s="4" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6358,7 +6369,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
@@ -6420,7 +6431,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.56"/>
@@ -6439,620 +6450,620 @@
       <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>306</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>309</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>312</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>314</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="9" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
+      <c r="A6" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>316</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="9" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>318</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="9" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>320</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="9" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>322</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="9" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="n">
+      <c r="A10" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>324</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="9" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
+      <c r="A11" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>326</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="9" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
+      <c r="A12" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>328</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
+      <c r="A13" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>330</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="9" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="n">
+      <c r="A14" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>332</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>308</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="9" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="n">
+      <c r="A15" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>334</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E15" s="8" t="n">
+      <c r="E15" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="9" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="n">
+      <c r="A16" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>336</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E16" s="8" t="n">
+      <c r="E16" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="9" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="n">
+      <c r="A17" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>338</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E17" s="8" t="n">
+      <c r="E17" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F17" s="8" t="n">
+      <c r="F17" s="9" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="n">
+      <c r="A18" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>340</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E18" s="8" t="n">
+      <c r="E18" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="8" t="n">
+      <c r="F18" s="9" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="n">
+      <c r="A19" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>342</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E19" s="8" t="n">
+      <c r="E19" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F19" s="8" t="n">
+      <c r="F19" s="9" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="n">
+      <c r="A20" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>344</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E20" s="8" t="n">
+      <c r="E20" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="9" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>346</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E21" s="8" t="n">
+      <c r="E21" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="8" t="n">
+      <c r="F21" s="9" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="n">
+      <c r="A22" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>348</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E22" s="8" t="n">
+      <c r="E22" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="8" t="n">
+      <c r="F22" s="9" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
+      <c r="A23" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>350</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E23" s="8" t="n">
+      <c r="E23" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F23" s="8" t="n">
+      <c r="F23" s="9" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="n">
+      <c r="A24" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>352</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E24" s="8" t="n">
+      <c r="E24" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F24" s="8" t="n">
+      <c r="F24" s="9" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="n">
+      <c r="A25" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>354</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E25" s="8" t="n">
+      <c r="E25" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F25" s="8" t="n">
+      <c r="F25" s="9" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>356</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E26" s="8" t="n">
+      <c r="E26" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F26" s="8" t="n">
+      <c r="F26" s="9" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>358</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E27" s="8" t="n">
+      <c r="E27" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="F27" s="8" t="n">
+      <c r="F27" s="9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>360</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E28" s="8" t="n">
+      <c r="E28" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="F28" s="8" t="n">
+      <c r="F28" s="9" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="n">
+      <c r="A29" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>362</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E29" s="8" t="n">
+      <c r="E29" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="F29" s="8" t="n">
+      <c r="F29" s="9" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>364</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E30" s="8" t="n">
+      <c r="E30" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="F30" s="8" t="n">
+      <c r="F30" s="9" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
+      <c r="A31" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>366</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="E31" s="8" t="n">
+      <c r="E31" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="F31" s="8" t="n">
+      <c r="F31" s="9" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>